<commit_message>
update Laporan and add Excel Solver
</commit_message>
<xml_diff>
--- a/dataset padi.xlsx
+++ b/dataset padi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Kuliah\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Kuliah\TRO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1C4F78-92A8-4687-B938-A7C898D4BD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A32B6F1-08B8-4AFD-A92D-D9DCCF8F69AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,9 +73,6 @@
     <t>JAWA BARAT</t>
   </si>
   <si>
-    <t>10 provinsi</t>
-  </si>
-  <si>
     <t>tahun 2025</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>5 provinsi</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -491,7 +491,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -509,7 +509,7 @@
     </row>
     <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -527,7 +527,7 @@
     </row>
     <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -560,7 +560,7 @@
         <v>9</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>10</v>
@@ -573,207 +573,245 @@
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2">
-        <v>100</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="1">
+        <v>100</v>
+      </c>
+      <c r="C4" s="1">
         <v>120</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>90</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>80</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>50</v>
       </c>
-      <c r="G4" s="2">
-        <v>100</v>
-      </c>
-      <c r="H4" s="2">
+      <c r="G4" s="1">
+        <v>100</v>
+      </c>
+      <c r="H4" s="1">
         <v>150</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>200</v>
       </c>
-      <c r="J4" s="2">
-        <v>100</v>
-      </c>
-      <c r="K4" s="2">
+      <c r="J4" s="1">
+        <v>100</v>
+      </c>
+      <c r="K4" s="1">
         <v>80</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>80</v>
       </c>
-      <c r="C5" s="2">
-        <v>100</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="1">
+        <v>100</v>
+      </c>
+      <c r="D5" s="1">
         <v>50</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>80</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>70</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>130</v>
       </c>
-      <c r="H5" s="2">
-        <v>100</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="H5" s="1">
+        <v>100</v>
+      </c>
+      <c r="I5" s="1">
         <v>120</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>90</v>
       </c>
-      <c r="K5" s="2">
-        <v>100</v>
-      </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="K5" s="1">
+        <v>100</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2">
-        <v>100</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="1">
+        <v>100</v>
+      </c>
+      <c r="C6" s="1">
         <v>80</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>30</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>20</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="G6" s="2">
-        <v>100</v>
-      </c>
-      <c r="H6" s="2">
-        <v>100</v>
-      </c>
-      <c r="I6" s="2">
-        <v>100</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="G6" s="1">
+        <v>100</v>
+      </c>
+      <c r="H6" s="1">
+        <v>100</v>
+      </c>
+      <c r="I6" s="1">
+        <v>100</v>
+      </c>
+      <c r="J6" s="1">
         <v>180</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <v>120</v>
       </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>150</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>40</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>0</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>50</v>
       </c>
-      <c r="F7" s="2">
-        <v>100</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="F7" s="1">
+        <v>100</v>
+      </c>
+      <c r="G7" s="1">
         <v>150</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>80</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>150</v>
       </c>
-      <c r="J7" s="2">
-        <v>100</v>
-      </c>
-      <c r="K7" s="2">
+      <c r="J7" s="1">
+        <v>100</v>
+      </c>
+      <c r="K7" s="1">
         <v>130</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>20</v>
       </c>
-      <c r="C8" s="2">
-        <v>100</v>
-      </c>
-      <c r="D8" s="2">
-        <v>100</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="C8" s="1">
+        <v>100</v>
+      </c>
+      <c r="D8" s="1">
+        <v>100</v>
+      </c>
+      <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="F8" s="2">
-        <v>100</v>
-      </c>
-      <c r="G8" s="2">
-        <v>100</v>
-      </c>
-      <c r="H8" s="2">
+      <c r="F8" s="1">
+        <v>100</v>
+      </c>
+      <c r="G8" s="1">
+        <v>100</v>
+      </c>
+      <c r="H8" s="1">
         <v>90</v>
       </c>
-      <c r="I8" s="2">
-        <v>100</v>
-      </c>
-      <c r="J8" s="2">
+      <c r="I8" s="1">
+        <v>100</v>
+      </c>
+      <c r="J8" s="1">
         <v>80</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <v>0</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1">
+        <f>SUM(B4:B8)</f>
+        <v>450</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" ref="C9:M9" si="0">SUM(C4:C8)</f>
+        <v>440</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>320</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>580</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="0"/>
+        <v>520</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>670</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="0"/>
+        <v>550</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="0"/>
+        <v>430</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
@@ -840,61 +878,18 @@
       <c r="N13" s="2"/>
     </row>
     <row r="14" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="2">
-        <f>SUM(B4:B13)</f>
-        <v>450</v>
-      </c>
-      <c r="C14" s="2">
-        <f>SUM(C4:C13)</f>
-        <v>440</v>
-      </c>
-      <c r="D14" s="2">
-        <f t="shared" ref="D14:N14" si="0">SUM(D4:D13)</f>
-        <v>270</v>
-      </c>
-      <c r="E14" s="2">
-        <f t="shared" si="0"/>
-        <v>230</v>
-      </c>
-      <c r="F14" s="2">
-        <f t="shared" si="0"/>
-        <v>320</v>
-      </c>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>580</v>
-      </c>
-      <c r="H14" s="2">
-        <f t="shared" si="0"/>
-        <v>520</v>
-      </c>
-      <c r="I14" s="2">
-        <f t="shared" si="0"/>
-        <v>670</v>
-      </c>
-      <c r="J14" s="2">
-        <f t="shared" si="0"/>
-        <v>550</v>
-      </c>
-      <c r="K14" s="2">
-        <f t="shared" si="0"/>
-        <v>430</v>
-      </c>
-      <c r="L14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>